<commit_message>
work on histograms, new data
</commit_message>
<xml_diff>
--- a/symm_groups.xlsx
+++ b/symm_groups.xlsx
@@ -12,15 +12,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="20">
-  <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>B</t>
-  </si>
-  <si>
-    <t>E</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="21">
+  <si>
+    <t>Arap</t>
+  </si>
+  <si>
+    <t>Bizans</t>
+  </si>
+  <si>
+    <t>Ermeni</t>
+  </si>
+  <si>
+    <t>Selçuk</t>
   </si>
   <si>
     <t>p1</t>
@@ -91,7 +94,7 @@
     <font>
       <sz val="12"/>
       <color indexed="8"/>
-      <name val="Helvetica Neue"/>
+      <name val="Helvetica"/>
     </font>
     <font>
       <sz val="13"/>
@@ -148,7 +151,7 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -158,22 +161,16 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="59" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="59" fontId="3" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="59" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -243,14 +240,14 @@
     </a:clrScheme>
     <a:fontScheme name="Office Theme">
       <a:majorFont>
-        <a:latin typeface="Helvetica Neue"/>
-        <a:ea typeface="Helvetica Neue"/>
-        <a:cs typeface="Helvetica Neue"/>
+        <a:latin typeface="Helvetica"/>
+        <a:ea typeface="Helvetica"/>
+        <a:cs typeface="Helvetica"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Helvetica Neue"/>
-        <a:ea typeface="Helvetica Neue"/>
-        <a:cs typeface="Helvetica Neue"/>
+        <a:latin typeface="Helvetica"/>
+        <a:ea typeface="Helvetica"/>
+        <a:cs typeface="Helvetica"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office Theme">
@@ -345,9 +342,9 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="20000" dir="5400000">
+            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="23000" dir="5400000">
               <a:srgbClr val="000000">
-                <a:alpha val="38000"/>
+                <a:alpha val="35000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
@@ -427,7 +424,7 @@
         </a:effectLst>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -455,10 +452,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Calibri"/>
-            <a:ea typeface="Calibri"/>
-            <a:cs typeface="Calibri"/>
-            <a:sym typeface="Calibri"/>
+            <a:latin typeface="Helvetica Neue"/>
+            <a:ea typeface="Helvetica Neue"/>
+            <a:cs typeface="Helvetica Neue"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -714,9 +711,9 @@
           <a:round/>
         </a:ln>
         <a:effectLst>
-          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="20000" dir="5400000">
+          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="23000" dir="5400000">
             <a:srgbClr val="000000">
-              <a:alpha val="38000"/>
+              <a:alpha val="35000"/>
             </a:srgbClr>
           </a:outerShdw>
         </a:effectLst>
@@ -1004,7 +1001,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1032,10 +1029,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Calibri"/>
-            <a:ea typeface="Calibri"/>
-            <a:cs typeface="Calibri"/>
-            <a:sym typeface="Calibri"/>
+            <a:latin typeface="Helvetica Neue"/>
+            <a:ea typeface="Helvetica Neue"/>
+            <a:cs typeface="Helvetica Neue"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -1286,14 +1283,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:S20"/>
+  <dimension ref="A1:R18"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.8333" defaultRowHeight="13" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="19" width="10.8516" style="1" customWidth="1"/>
-    <col min="20" max="256" width="10.8516" style="1" customWidth="1"/>
+    <col min="1" max="1" width="10.8516" style="1" customWidth="1"/>
+    <col min="2" max="2" width="10.8516" style="1" customWidth="1"/>
+    <col min="3" max="3" width="10.8516" style="1" customWidth="1"/>
+    <col min="4" max="4" width="10.8516" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10.8516" style="1" customWidth="1"/>
+    <col min="6" max="6" width="10.8516" style="1" customWidth="1"/>
+    <col min="7" max="7" width="10.8516" style="1" customWidth="1"/>
+    <col min="8" max="8" width="10.8516" style="1" customWidth="1"/>
+    <col min="9" max="9" width="10.8516" style="1" customWidth="1"/>
+    <col min="10" max="10" width="10.8516" style="1" customWidth="1"/>
+    <col min="11" max="11" width="10.8516" style="1" customWidth="1"/>
+    <col min="12" max="12" width="10.8516" style="1" customWidth="1"/>
+    <col min="13" max="13" width="10.8516" style="1" customWidth="1"/>
+    <col min="14" max="14" width="10.8516" style="1" customWidth="1"/>
+    <col min="15" max="15" width="10.8516" style="1" customWidth="1"/>
+    <col min="16" max="16" width="10.8516" style="1" customWidth="1"/>
+    <col min="17" max="17" width="10.8516" style="1" customWidth="1"/>
+    <col min="18" max="18" width="10.8516" style="1" customWidth="1"/>
+    <col min="19" max="256" width="10.8516" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="15" customHeight="1">
@@ -1307,562 +1321,538 @@
       <c r="D1" t="s" s="3">
         <v>2</v>
       </c>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
-      <c r="L1" s="4"/>
-      <c r="M1" s="4"/>
-      <c r="N1" s="4"/>
-      <c r="O1" s="4"/>
-      <c r="P1" s="4"/>
-      <c r="Q1" s="4"/>
-      <c r="R1" s="2"/>
-      <c r="S1" s="4"/>
+      <c r="E1" t="s" s="3">
+        <v>3</v>
+      </c>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
+      <c r="P1" s="3"/>
+      <c r="Q1" s="2"/>
+      <c r="R1" s="4"/>
     </row>
     <row r="2" ht="15" customHeight="1">
-      <c r="A2" t="s" s="5">
-        <v>3</v>
-      </c>
-      <c r="B2" s="6">
+      <c r="A2" t="s" s="3">
+        <v>4</v>
+      </c>
+      <c r="B2" s="5">
         <v>0</v>
       </c>
-      <c r="C2" s="6">
+      <c r="C2" s="5">
         <v>14.04</v>
       </c>
-      <c r="D2" s="6">
+      <c r="D2" s="5">
         <v>5.6</v>
       </c>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4"/>
-      <c r="L2" s="4"/>
-      <c r="M2" s="4"/>
-      <c r="N2" s="4"/>
-      <c r="O2" s="4"/>
-      <c r="P2" s="4"/>
-      <c r="Q2" s="4"/>
+      <c r="E2" s="5">
+        <v>0.27</v>
+      </c>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+      <c r="O2" s="2"/>
+      <c r="P2" s="2"/>
+      <c r="Q2" s="2"/>
       <c r="R2" s="2"/>
-      <c r="S2" s="4"/>
     </row>
     <row r="3" ht="15" customHeight="1">
-      <c r="A3" t="s" s="5">
-        <v>4</v>
-      </c>
-      <c r="B3" s="6">
+      <c r="A3" t="s" s="3">
+        <v>5</v>
+      </c>
+      <c r="B3" s="5">
         <v>0.3</v>
       </c>
-      <c r="C3" s="6">
+      <c r="C3" s="5">
         <v>9.65</v>
       </c>
-      <c r="D3" s="6">
+      <c r="D3" s="5">
         <v>0</v>
       </c>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4"/>
-      <c r="K3" s="4"/>
-      <c r="L3" s="4"/>
-      <c r="M3" s="4"/>
-      <c r="N3" s="4"/>
-      <c r="O3" s="4"/>
-      <c r="P3" s="4"/>
-      <c r="Q3" s="4"/>
+      <c r="E3" s="5">
+        <v>0</v>
+      </c>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+      <c r="O3" s="2"/>
+      <c r="P3" s="2"/>
+      <c r="Q3" s="2"/>
       <c r="R3" s="2"/>
-      <c r="S3" s="4"/>
     </row>
     <row r="4" ht="15" customHeight="1">
-      <c r="A4" t="s" s="5">
-        <v>5</v>
-      </c>
-      <c r="B4" s="6">
+      <c r="A4" t="s" s="3">
+        <v>6</v>
+      </c>
+      <c r="B4" s="5">
         <v>0</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C4" s="5">
         <v>0.88</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4" s="5">
         <v>0</v>
       </c>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4"/>
-      <c r="K4" s="4"/>
-      <c r="L4" s="4"/>
-      <c r="M4" s="4"/>
-      <c r="N4" s="4"/>
-      <c r="O4" s="4"/>
-      <c r="P4" s="4"/>
-      <c r="Q4" s="4"/>
+      <c r="E4" s="5">
+        <v>0</v>
+      </c>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
+      <c r="O4" s="2"/>
+      <c r="P4" s="2"/>
+      <c r="Q4" s="2"/>
       <c r="R4" s="2"/>
-      <c r="S4" s="4"/>
     </row>
     <row r="5" ht="15" customHeight="1">
-      <c r="A5" t="s" s="5">
-        <v>6</v>
-      </c>
-      <c r="B5" s="6">
+      <c r="A5" t="s" s="3">
+        <v>7</v>
+      </c>
+      <c r="B5" s="5">
         <v>0</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="5">
         <v>4.39</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="5">
         <v>2.4</v>
       </c>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
-      <c r="J5" s="4"/>
-      <c r="K5" s="4"/>
-      <c r="L5" s="4"/>
-      <c r="M5" s="4"/>
-      <c r="N5" s="4"/>
-      <c r="O5" s="4"/>
-      <c r="P5" s="4"/>
-      <c r="Q5" s="4"/>
+      <c r="E5" s="5">
+        <v>0.55</v>
+      </c>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
+      <c r="O5" s="2"/>
+      <c r="P5" s="2"/>
+      <c r="Q5" s="2"/>
       <c r="R5" s="2"/>
-      <c r="S5" s="4"/>
     </row>
     <row r="6" ht="15" customHeight="1">
-      <c r="A6" t="s" s="5">
-        <v>7</v>
-      </c>
-      <c r="B6" s="6">
+      <c r="A6" t="s" s="3">
+        <v>8</v>
+      </c>
+      <c r="B6" s="5">
         <v>0.6</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6" s="5">
         <v>2.63</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6" s="5">
         <v>4</v>
       </c>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
-      <c r="J6" s="4"/>
-      <c r="K6" s="4"/>
-      <c r="L6" s="4"/>
-      <c r="M6" s="4"/>
-      <c r="N6" s="4"/>
-      <c r="O6" s="4"/>
-      <c r="P6" s="4"/>
-      <c r="Q6" s="4"/>
+      <c r="E6" s="5">
+        <v>1.1</v>
+      </c>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
+      <c r="O6" s="2"/>
+      <c r="P6" s="2"/>
+      <c r="Q6" s="2"/>
       <c r="R6" s="2"/>
-      <c r="S6" s="4"/>
     </row>
     <row r="7" ht="15" customHeight="1">
-      <c r="A7" t="s" s="5">
-        <v>8</v>
-      </c>
-      <c r="B7" s="6">
+      <c r="A7" t="s" s="3">
+        <v>9</v>
+      </c>
+      <c r="B7" s="5">
         <v>3.9</v>
       </c>
-      <c r="C7" s="6">
+      <c r="C7" s="5">
         <v>9.65</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D7" s="5">
         <v>1.6</v>
       </c>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="4"/>
-      <c r="J7" s="4"/>
-      <c r="K7" s="4"/>
-      <c r="L7" s="4"/>
-      <c r="M7" s="4"/>
-      <c r="N7" s="4"/>
-      <c r="O7" s="4"/>
-      <c r="P7" s="4"/>
-      <c r="Q7" s="4"/>
-      <c r="R7" s="2"/>
-      <c r="S7" s="4"/>
+      <c r="E7" s="5">
+        <v>8.789999999999999</v>
+      </c>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
+      <c r="O7" s="2"/>
+      <c r="P7" s="2"/>
+      <c r="Q7" s="2"/>
+      <c r="R7" s="6"/>
     </row>
     <row r="8" ht="15" customHeight="1">
-      <c r="A8" t="s" s="5">
-        <v>9</v>
-      </c>
-      <c r="B8" s="6">
+      <c r="A8" t="s" s="3">
+        <v>10</v>
+      </c>
+      <c r="B8" s="5">
         <v>0.3</v>
       </c>
-      <c r="C8" s="6">
+      <c r="C8" s="5">
         <v>5.26</v>
       </c>
-      <c r="D8" s="6">
+      <c r="D8" s="5">
         <v>0</v>
       </c>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="4"/>
-      <c r="J8" s="4"/>
-      <c r="K8" s="4"/>
-      <c r="L8" s="4"/>
-      <c r="M8" s="4"/>
-      <c r="N8" s="4"/>
-      <c r="O8" s="4"/>
-      <c r="P8" s="4"/>
-      <c r="Q8" s="4"/>
+      <c r="E8" s="5">
+        <v>0.82</v>
+      </c>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="2"/>
+      <c r="O8" s="2"/>
+      <c r="P8" s="2"/>
+      <c r="Q8" s="2"/>
       <c r="R8" s="2"/>
-      <c r="S8" s="4"/>
     </row>
     <row r="9" ht="15" customHeight="1">
-      <c r="A9" t="s" s="5">
-        <v>10</v>
-      </c>
-      <c r="B9" s="6">
+      <c r="A9" t="s" s="3">
+        <v>11</v>
+      </c>
+      <c r="B9" s="5">
         <v>0</v>
       </c>
-      <c r="C9" s="6">
+      <c r="C9" s="5">
         <v>0.88</v>
       </c>
-      <c r="D9" s="6">
+      <c r="D9" s="5">
         <v>6.4</v>
       </c>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
-      <c r="I9" s="4"/>
-      <c r="J9" s="4"/>
-      <c r="K9" s="4"/>
-      <c r="L9" s="4"/>
-      <c r="M9" s="4"/>
-      <c r="N9" s="4"/>
-      <c r="O9" s="4"/>
-      <c r="P9" s="4"/>
-      <c r="Q9" s="4"/>
+      <c r="E9" s="5">
+        <v>0.55</v>
+      </c>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
+      <c r="N9" s="2"/>
+      <c r="O9" s="2"/>
+      <c r="P9" s="2"/>
+      <c r="Q9" s="2"/>
       <c r="R9" s="2"/>
-      <c r="S9" s="4"/>
     </row>
     <row r="10" ht="15" customHeight="1">
-      <c r="A10" t="s" s="5">
-        <v>11</v>
-      </c>
-      <c r="B10" s="6">
+      <c r="A10" t="s" s="3">
+        <v>12</v>
+      </c>
+      <c r="B10" s="5">
         <v>9.5</v>
       </c>
-      <c r="C10" s="6">
+      <c r="C10" s="5">
         <v>3.51</v>
       </c>
-      <c r="D10" s="6">
+      <c r="D10" s="5">
         <v>1.6</v>
       </c>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
-      <c r="I10" s="4"/>
-      <c r="J10" s="4"/>
-      <c r="K10" s="4"/>
-      <c r="L10" s="4"/>
-      <c r="M10" s="4"/>
-      <c r="N10" s="4"/>
-      <c r="O10" s="4"/>
-      <c r="P10" s="4"/>
-      <c r="Q10" s="4"/>
+      <c r="E10" s="5">
+        <v>8.52</v>
+      </c>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
+      <c r="L10" s="2"/>
+      <c r="M10" s="2"/>
+      <c r="N10" s="2"/>
+      <c r="O10" s="2"/>
+      <c r="P10" s="2"/>
+      <c r="Q10" s="2"/>
       <c r="R10" s="2"/>
-      <c r="S10" s="4"/>
     </row>
     <row r="11" ht="15" customHeight="1">
-      <c r="A11" t="s" s="5">
-        <v>12</v>
-      </c>
-      <c r="B11" s="6">
+      <c r="A11" t="s" s="3">
+        <v>13</v>
+      </c>
+      <c r="B11" s="5">
         <v>0.3</v>
       </c>
-      <c r="C11" s="6">
+      <c r="C11" s="5">
         <v>0</v>
       </c>
-      <c r="D11" s="6">
+      <c r="D11" s="5">
         <v>0.8</v>
       </c>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4"/>
-      <c r="I11" s="4"/>
-      <c r="J11" s="4"/>
-      <c r="K11" s="4"/>
-      <c r="L11" s="4"/>
-      <c r="M11" s="4"/>
-      <c r="N11" s="4"/>
-      <c r="O11" s="4"/>
-      <c r="P11" s="4"/>
-      <c r="Q11" s="4"/>
+      <c r="E11" s="5">
+        <v>0.82</v>
+      </c>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
+      <c r="L11" s="2"/>
+      <c r="M11" s="2"/>
+      <c r="N11" s="2"/>
+      <c r="O11" s="2"/>
+      <c r="P11" s="2"/>
+      <c r="Q11" s="2"/>
       <c r="R11" s="2"/>
-      <c r="S11" s="4"/>
     </row>
     <row r="12" ht="15" customHeight="1">
-      <c r="A12" t="s" s="5">
-        <v>13</v>
-      </c>
-      <c r="B12" s="6">
+      <c r="A12" t="s" s="3">
+        <v>14</v>
+      </c>
+      <c r="B12" s="5">
         <v>0</v>
       </c>
-      <c r="C12" s="6">
+      <c r="C12" s="5">
         <v>0</v>
       </c>
-      <c r="D12" s="6">
+      <c r="D12" s="5">
         <v>0</v>
       </c>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="4"/>
-      <c r="I12" s="4"/>
-      <c r="J12" s="4"/>
-      <c r="K12" s="4"/>
-      <c r="L12" s="4"/>
-      <c r="M12" s="4"/>
-      <c r="N12" s="4"/>
-      <c r="O12" s="4"/>
-      <c r="P12" s="4"/>
-      <c r="Q12" s="4"/>
+      <c r="E12" s="5">
+        <v>0</v>
+      </c>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
+      <c r="L12" s="2"/>
+      <c r="M12" s="2"/>
+      <c r="N12" s="2"/>
+      <c r="O12" s="2"/>
+      <c r="P12" s="2"/>
+      <c r="Q12" s="2"/>
       <c r="R12" s="2"/>
-      <c r="S12" s="4"/>
     </row>
     <row r="13" ht="15" customHeight="1">
-      <c r="A13" t="s" s="5">
-        <v>14</v>
-      </c>
-      <c r="B13" s="6">
+      <c r="A13" t="s" s="3">
+        <v>15</v>
+      </c>
+      <c r="B13" s="5">
         <v>1.2</v>
       </c>
-      <c r="C13" s="6">
+      <c r="C13" s="5">
         <v>0</v>
       </c>
-      <c r="D13" s="6">
+      <c r="D13" s="5">
         <v>2.4</v>
       </c>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
-      <c r="I13" s="4"/>
-      <c r="J13" s="4"/>
-      <c r="K13" s="4"/>
-      <c r="L13" s="4"/>
-      <c r="M13" s="4"/>
-      <c r="N13" s="4"/>
-      <c r="O13" s="4"/>
-      <c r="P13" s="4"/>
-      <c r="Q13" s="4"/>
+      <c r="E13" s="5">
+        <v>1.92</v>
+      </c>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
+      <c r="K13" s="2"/>
+      <c r="L13" s="2"/>
+      <c r="M13" s="2"/>
+      <c r="N13" s="2"/>
+      <c r="O13" s="2"/>
+      <c r="P13" s="2"/>
+      <c r="Q13" s="2"/>
       <c r="R13" s="2"/>
-      <c r="S13" s="4"/>
     </row>
     <row r="14" ht="15" customHeight="1">
-      <c r="A14" t="s" s="5">
-        <v>15</v>
-      </c>
-      <c r="B14" s="6">
+      <c r="A14" t="s" s="3">
+        <v>16</v>
+      </c>
+      <c r="B14" s="5">
         <v>2.9</v>
       </c>
-      <c r="C14" s="6">
+      <c r="C14" s="5">
         <v>1.75</v>
       </c>
-      <c r="D14" s="6">
+      <c r="D14" s="5">
         <v>49.6</v>
       </c>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
-      <c r="I14" s="4"/>
-      <c r="J14" s="4"/>
-      <c r="K14" s="4"/>
-      <c r="L14" s="4"/>
-      <c r="M14" s="4"/>
-      <c r="N14" s="4"/>
-      <c r="O14" s="4"/>
-      <c r="P14" s="4"/>
-      <c r="Q14" s="4"/>
-      <c r="R14" s="2"/>
-      <c r="S14" s="4"/>
+      <c r="E14" s="5">
+        <v>8.24</v>
+      </c>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2"/>
+      <c r="L14" s="2"/>
+      <c r="M14" s="2"/>
+      <c r="N14" s="2"/>
+      <c r="O14" s="2"/>
+      <c r="P14" s="2"/>
+      <c r="Q14" s="2"/>
+      <c r="R14" s="6"/>
     </row>
     <row r="15" ht="15" customHeight="1">
-      <c r="A15" t="s" s="5">
-        <v>16</v>
-      </c>
-      <c r="B15" s="6">
+      <c r="A15" t="s" s="3">
+        <v>17</v>
+      </c>
+      <c r="B15" s="5">
         <v>47.8</v>
       </c>
-      <c r="C15" s="6">
+      <c r="C15" s="5">
         <v>35.09</v>
       </c>
-      <c r="D15" s="6">
+      <c r="D15" s="5">
         <v>12.8</v>
       </c>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
-      <c r="H15" s="4"/>
-      <c r="I15" s="4"/>
-      <c r="J15" s="4"/>
-      <c r="K15" s="4"/>
-      <c r="L15" s="4"/>
-      <c r="M15" s="4"/>
-      <c r="N15" s="4"/>
-      <c r="O15" s="4"/>
-      <c r="P15" s="4"/>
-      <c r="Q15" s="4"/>
+      <c r="E15" s="5">
+        <v>27.75</v>
+      </c>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="2"/>
+      <c r="K15" s="2"/>
+      <c r="L15" s="2"/>
+      <c r="M15" s="2"/>
+      <c r="N15" s="2"/>
+      <c r="O15" s="2"/>
+      <c r="P15" s="2"/>
+      <c r="Q15" s="2"/>
       <c r="R15" s="2"/>
-      <c r="S15" s="4"/>
     </row>
     <row r="16" ht="15" customHeight="1">
-      <c r="A16" t="s" s="5">
-        <v>17</v>
-      </c>
-      <c r="B16" s="6">
+      <c r="A16" t="s" s="3">
+        <v>18</v>
+      </c>
+      <c r="B16" s="5">
         <v>6.4</v>
       </c>
-      <c r="C16" s="6">
+      <c r="C16" s="5">
         <v>11.4</v>
       </c>
-      <c r="D16" s="6">
+      <c r="D16" s="5">
         <v>4</v>
       </c>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
-      <c r="G16" s="4"/>
-      <c r="H16" s="4"/>
-      <c r="I16" s="4"/>
-      <c r="J16" s="4"/>
-      <c r="K16" s="4"/>
-      <c r="L16" s="4"/>
-      <c r="M16" s="4"/>
-      <c r="N16" s="4"/>
-      <c r="O16" s="4"/>
-      <c r="P16" s="4"/>
-      <c r="Q16" s="4"/>
+      <c r="E16" s="5">
+        <v>5.22</v>
+      </c>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2"/>
+      <c r="K16" s="2"/>
+      <c r="L16" s="2"/>
+      <c r="M16" s="2"/>
+      <c r="N16" s="2"/>
+      <c r="O16" s="2"/>
+      <c r="P16" s="2"/>
+      <c r="Q16" s="2"/>
       <c r="R16" s="2"/>
-      <c r="S16" s="4"/>
     </row>
     <row r="17" ht="15" customHeight="1">
-      <c r="A17" t="s" s="5">
-        <v>18</v>
-      </c>
-      <c r="B17" s="6">
+      <c r="A17" t="s" s="3">
+        <v>19</v>
+      </c>
+      <c r="B17" s="5">
         <v>4.2</v>
       </c>
-      <c r="C17" s="6">
+      <c r="C17" s="5">
         <v>0.88</v>
       </c>
-      <c r="D17" s="6">
+      <c r="D17" s="5">
         <v>4.8</v>
       </c>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
-      <c r="G17" s="4"/>
-      <c r="H17" s="4"/>
-      <c r="I17" s="4"/>
-      <c r="J17" s="4"/>
-      <c r="K17" s="4"/>
-      <c r="L17" s="4"/>
-      <c r="M17" s="4"/>
-      <c r="N17" s="4"/>
-      <c r="O17" s="4"/>
-      <c r="P17" s="4"/>
-      <c r="Q17" s="4"/>
+      <c r="E17" s="5">
+        <v>7.97</v>
+      </c>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+      <c r="I17" s="2"/>
+      <c r="J17" s="2"/>
+      <c r="K17" s="2"/>
+      <c r="L17" s="2"/>
+      <c r="M17" s="2"/>
+      <c r="N17" s="2"/>
+      <c r="O17" s="2"/>
+      <c r="P17" s="2"/>
+      <c r="Q17" s="2"/>
       <c r="R17" s="2"/>
-      <c r="S17" s="4"/>
     </row>
     <row r="18" ht="15" customHeight="1">
-      <c r="A18" t="s" s="5">
-        <v>19</v>
-      </c>
-      <c r="B18" s="6">
+      <c r="A18" t="s" s="3">
+        <v>20</v>
+      </c>
+      <c r="B18" s="5">
         <v>22.2</v>
       </c>
-      <c r="C18" s="6">
+      <c r="C18" s="5">
         <v>0</v>
       </c>
-      <c r="D18" s="6">
+      <c r="D18" s="5">
         <v>4</v>
       </c>
-      <c r="E18" s="4"/>
-      <c r="F18" s="4"/>
-      <c r="G18" s="4"/>
-      <c r="H18" s="4"/>
-      <c r="I18" s="4"/>
-      <c r="J18" s="4"/>
-      <c r="K18" s="4"/>
-      <c r="L18" s="4"/>
-      <c r="M18" s="4"/>
-      <c r="N18" s="4"/>
-      <c r="O18" s="4"/>
-      <c r="P18" s="4"/>
-      <c r="Q18" s="4"/>
+      <c r="E18" s="5">
+        <v>27.47</v>
+      </c>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
+      <c r="J18" s="2"/>
+      <c r="K18" s="2"/>
+      <c r="L18" s="2"/>
+      <c r="M18" s="2"/>
+      <c r="N18" s="2"/>
+      <c r="O18" s="2"/>
+      <c r="P18" s="2"/>
+      <c r="Q18" s="2"/>
       <c r="R18" s="2"/>
-      <c r="S18" s="4"/>
-    </row>
-    <row r="19" ht="15" customHeight="1">
-      <c r="A19" s="2"/>
-      <c r="B19" s="4"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="4"/>
-      <c r="G19" s="4"/>
-      <c r="H19" s="4"/>
-      <c r="I19" s="4"/>
-      <c r="J19" s="4"/>
-      <c r="K19" s="4"/>
-      <c r="L19" s="4"/>
-      <c r="M19" s="4"/>
-      <c r="N19" s="4"/>
-      <c r="O19" s="4"/>
-      <c r="P19" s="4"/>
-      <c r="Q19" s="4"/>
-      <c r="R19" s="2"/>
-      <c r="S19" s="4"/>
-    </row>
-    <row r="20" ht="15" customHeight="1">
-      <c r="A20" s="7"/>
-      <c r="B20" s="4"/>
-      <c r="C20" s="4"/>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="4"/>
-      <c r="G20" s="8"/>
-      <c r="H20" s="4"/>
-      <c r="I20" s="4"/>
-      <c r="J20" s="4"/>
-      <c r="K20" s="4"/>
-      <c r="L20" s="4"/>
-      <c r="M20" s="4"/>
-      <c r="N20" s="8"/>
-      <c r="O20" s="4"/>
-      <c r="P20" s="4"/>
-      <c r="Q20" s="4"/>
-      <c r="R20" s="2"/>
-      <c r="S20" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="92" useFirstPageNumber="0" orientation="landscape" pageOrder="downThenOver"/>
   <headerFooter>
-    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
+    <oddFooter>&amp;C&amp;"Helvetica,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
yeni peterson datalari ile
</commit_message>
<xml_diff>
--- a/symm_groups.xlsx
+++ b/symm_groups.xlsx
@@ -12,15 +12,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="21">
-  <si>
-    <t>Moslem Arabs</t>
-  </si>
-  <si>
-    <t>Eastern Roman Empire</t>
-  </si>
-  <si>
-    <t>Armenia</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="65">
+  <si>
+    <t>Andalusia</t>
+  </si>
+  <si>
+    <t>ME Arabs</t>
+  </si>
+  <si>
+    <t>Eastern Roman</t>
+  </si>
+  <si>
+    <t>Armenian</t>
   </si>
   <si>
     <t>Seljuks</t>
@@ -29,33 +32,108 @@
     <t>p1</t>
   </si>
   <si>
+    <t>0.00</t>
+  </si>
+  <si>
+    <t>14.04</t>
+  </si>
+  <si>
+    <t>0.8</t>
+  </si>
+  <si>
+    <t>0.27</t>
+  </si>
+  <si>
     <t>p1m1</t>
   </si>
   <si>
+    <t>9.65</t>
+  </si>
+  <si>
+    <t>4.9</t>
+  </si>
+  <si>
     <t>p1g1</t>
   </si>
   <si>
+    <t>0.88</t>
+  </si>
+  <si>
     <t>c1m1</t>
   </si>
   <si>
+    <t>4.39</t>
+  </si>
+  <si>
+    <t>2.4</t>
+  </si>
+  <si>
+    <t>0.55</t>
+  </si>
+  <si>
     <t>p211</t>
   </si>
   <si>
+    <t>2.63</t>
+  </si>
+  <si>
+    <t>1.1</t>
+  </si>
+  <si>
     <t>p2mm</t>
   </si>
   <si>
+    <t>2.88</t>
+  </si>
+  <si>
+    <t>5.75</t>
+  </si>
+  <si>
+    <t>5.7</t>
+  </si>
+  <si>
+    <t>8.79</t>
+  </si>
+  <si>
     <t>p2mg</t>
   </si>
   <si>
+    <t>0.44</t>
+  </si>
+  <si>
+    <t>5.26</t>
+  </si>
+  <si>
+    <t>0.82</t>
+  </si>
+  <si>
     <t>p2gg</t>
   </si>
   <si>
     <t>c2mm</t>
   </si>
   <si>
+    <t>1.92</t>
+  </si>
+  <si>
+    <t>15.93</t>
+  </si>
+  <si>
+    <t>3.51</t>
+  </si>
+  <si>
+    <t>1.6</t>
+  </si>
+  <si>
+    <t>8.52</t>
+  </si>
+  <si>
     <t>p3</t>
   </si>
   <si>
+    <t>0.96</t>
+  </si>
+  <si>
     <t>p3m1</t>
   </si>
   <si>
@@ -65,16 +143,70 @@
     <t>p4</t>
   </si>
   <si>
+    <t>1.75</t>
+  </si>
+  <si>
+    <t>12.2</t>
+  </si>
+  <si>
+    <t>8.24</t>
+  </si>
+  <si>
     <t>p4mm</t>
   </si>
   <si>
+    <t>76.92</t>
+  </si>
+  <si>
+    <t>33.19</t>
+  </si>
+  <si>
+    <t>35.09</t>
+  </si>
+  <si>
+    <t>54.5</t>
+  </si>
+  <si>
+    <t>27.75</t>
+  </si>
+  <si>
     <t>p4gm</t>
   </si>
   <si>
+    <t>5.77</t>
+  </si>
+  <si>
+    <t>5.31</t>
+  </si>
+  <si>
+    <t>11.4</t>
+  </si>
+  <si>
+    <t>5.22</t>
+  </si>
+  <si>
     <t>p6</t>
   </si>
   <si>
+    <t>2.65</t>
+  </si>
+  <si>
+    <t>7.97</t>
+  </si>
+  <si>
     <t>p6mm</t>
+  </si>
+  <si>
+    <t>8.65</t>
+  </si>
+  <si>
+    <t>35.84</t>
+  </si>
+  <si>
+    <t>6.6</t>
+  </si>
+  <si>
+    <t>27.47</t>
   </si>
 </sst>
 </file>
@@ -85,7 +217,7 @@
     <numFmt numFmtId="0" formatCode="General"/>
     <numFmt numFmtId="59" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -94,12 +226,23 @@
     <font>
       <sz val="12"/>
       <color indexed="8"/>
-      <name val="Helvetica"/>
+      <name val="Helvetica Neue"/>
     </font>
     <font>
       <sz val="13"/>
       <color indexed="8"/>
       <name val="Verdana"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <sz val="24"/>
+      <color indexed="8"/>
+      <name val="Verdana"/>
+    </font>
+    <font>
+      <sz val="24"/>
+      <color indexed="8"/>
+      <name val="Times"/>
     </font>
     <font>
       <b val="1"/>
@@ -117,17 +260,47 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="9"/>
+        <fgColor indexed="11"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="4">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="9"/>
+      </left>
+      <right style="thin">
+        <color indexed="9"/>
+      </right>
+      <top style="thin">
+        <color indexed="9"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="9"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="9"/>
+      </left>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -145,81 +318,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="10"/>
-      </left>
-      <right style="thin">
-        <color indexed="11"/>
-      </right>
-      <top style="thin">
-        <color indexed="11"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="11"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="11"/>
-      </left>
-      <right style="thin">
-        <color indexed="11"/>
-      </right>
-      <top style="thin">
-        <color indexed="11"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="11"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="12"/>
-      </left>
-      <right style="thin">
-        <color indexed="12"/>
-      </right>
-      <top style="thin">
-        <color indexed="10"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="12"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="12"/>
-      </left>
-      <right style="thin">
-        <color indexed="11"/>
-      </right>
-      <top style="thin">
-        <color indexed="11"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="11"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="12"/>
-      </left>
-      <right style="thin">
-        <color indexed="12"/>
-      </right>
-      <top style="thin">
-        <color indexed="12"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="12"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
@@ -233,34 +331,34 @@
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="49" fontId="3" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="59" fontId="0" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="right" vertical="bottom" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="59" fontId="3" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="59" fontId="5" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -280,10 +378,9 @@
       <rgbColor rgb="ffff00ff"/>
       <rgbColor rgb="ff00ffff"/>
       <rgbColor rgb="ff000000"/>
+      <rgbColor rgb="ffcccccc"/>
+      <rgbColor rgb="ffaaaaaa"/>
       <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffcacaca"/>
-      <rgbColor rgb="ffaaaaaa"/>
-      <rgbColor rgb="ffcacaca"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -332,14 +429,14 @@
     </a:clrScheme>
     <a:fontScheme name="Office Theme">
       <a:majorFont>
-        <a:latin typeface="Helvetica"/>
-        <a:ea typeface="Helvetica"/>
-        <a:cs typeface="Helvetica"/>
+        <a:latin typeface="Helvetica Neue"/>
+        <a:ea typeface="Helvetica Neue"/>
+        <a:cs typeface="Helvetica Neue"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Helvetica"/>
-        <a:ea typeface="Helvetica"/>
-        <a:cs typeface="Helvetica"/>
+        <a:latin typeface="Helvetica Neue"/>
+        <a:ea typeface="Helvetica Neue"/>
+        <a:cs typeface="Helvetica Neue"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office Theme">
@@ -434,9 +531,9 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="23000" dir="5400000">
+            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="20000" dir="5400000">
               <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
+                <a:alpha val="38000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
@@ -516,7 +613,7 @@
         </a:effectLst>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -544,10 +641,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Helvetica Neue"/>
-            <a:ea typeface="Helvetica Neue"/>
-            <a:cs typeface="Helvetica Neue"/>
-            <a:sym typeface="Helvetica Neue"/>
+            <a:latin typeface="Calibri"/>
+            <a:ea typeface="Calibri"/>
+            <a:cs typeface="Calibri"/>
+            <a:sym typeface="Calibri"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -803,9 +900,9 @@
           <a:round/>
         </a:ln>
         <a:effectLst>
-          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="23000" dir="5400000">
+          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="20000" dir="5400000">
             <a:srgbClr val="000000">
-              <a:alpha val="35000"/>
+              <a:alpha val="38000"/>
             </a:srgbClr>
           </a:outerShdw>
         </a:effectLst>
@@ -1093,7 +1190,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1121,10 +1218,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Helvetica Neue"/>
-            <a:ea typeface="Helvetica Neue"/>
-            <a:cs typeface="Helvetica Neue"/>
-            <a:sym typeface="Helvetica Neue"/>
+            <a:latin typeface="Calibri"/>
+            <a:ea typeface="Calibri"/>
+            <a:cs typeface="Calibri"/>
+            <a:sym typeface="Calibri"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -1375,43 +1472,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AA18"/>
+  <dimension ref="A1:R18"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.8333" defaultRowHeight="13" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="10.8516" style="1" customWidth="1"/>
-    <col min="2" max="2" width="10.8516" style="1" customWidth="1"/>
-    <col min="3" max="3" width="10.8516" style="1" customWidth="1"/>
-    <col min="4" max="4" width="10.8516" style="1" customWidth="1"/>
-    <col min="5" max="5" width="10.8516" style="1" customWidth="1"/>
-    <col min="6" max="6" width="10.8516" style="1" customWidth="1"/>
-    <col min="7" max="7" width="10.8516" style="1" customWidth="1"/>
-    <col min="8" max="8" width="10.8516" style="1" customWidth="1"/>
-    <col min="9" max="9" width="10.8516" style="1" customWidth="1"/>
-    <col min="10" max="10" width="10.8516" style="1" customWidth="1"/>
-    <col min="11" max="11" width="10.8516" style="1" customWidth="1"/>
-    <col min="12" max="12" width="10.8516" style="1" customWidth="1"/>
-    <col min="13" max="13" width="10.8516" style="1" customWidth="1"/>
-    <col min="14" max="14" width="10.8516" style="1" customWidth="1"/>
-    <col min="15" max="15" width="10.8516" style="1" customWidth="1"/>
-    <col min="16" max="16" width="10.8516" style="1" customWidth="1"/>
-    <col min="17" max="17" width="10.8516" style="1" customWidth="1"/>
-    <col min="18" max="18" width="10.8516" style="1" customWidth="1"/>
-    <col min="19" max="19" width="10.8516" style="1" customWidth="1"/>
-    <col min="20" max="20" width="10.8516" style="1" customWidth="1"/>
-    <col min="21" max="21" width="10.8516" style="1" customWidth="1"/>
-    <col min="22" max="22" width="10.8516" style="1" customWidth="1"/>
-    <col min="23" max="23" width="10.8516" style="1" customWidth="1"/>
-    <col min="24" max="24" width="10.8516" style="1" customWidth="1"/>
-    <col min="25" max="25" width="10.8516" style="1" customWidth="1"/>
-    <col min="26" max="26" width="10.8516" style="1" customWidth="1"/>
-    <col min="27" max="27" width="10.8516" style="1" customWidth="1"/>
-    <col min="28" max="256" width="10.8516" style="1" customWidth="1"/>
+    <col min="1" max="18" width="10.8516" style="1" customWidth="1"/>
+    <col min="19" max="256" width="10.8516" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15" customHeight="1">
+    <row r="1" ht="30" customHeight="1">
       <c r="A1" s="2"/>
       <c r="B1" t="s" s="3">
         <v>0</v>
@@ -1425,8 +1496,10 @@
       <c r="E1" t="s" s="3">
         <v>3</v>
       </c>
-      <c r="F1" s="4"/>
-      <c r="G1" s="5"/>
+      <c r="F1" t="s" s="3">
+        <v>4</v>
+      </c>
+      <c r="G1" s="4"/>
       <c r="H1" s="5"/>
       <c r="I1" s="5"/>
       <c r="J1" s="5"/>
@@ -1437,35 +1510,28 @@
       <c r="O1" s="5"/>
       <c r="P1" s="5"/>
       <c r="Q1" s="5"/>
-      <c r="R1" s="5"/>
-      <c r="S1" s="5"/>
-      <c r="T1" s="5"/>
-      <c r="U1" s="5"/>
-      <c r="V1" s="5"/>
-      <c r="W1" s="5"/>
-      <c r="X1" s="5"/>
-      <c r="Y1" s="5"/>
-      <c r="Z1" s="5"/>
-      <c r="AA1" s="5"/>
+      <c r="R1" s="6"/>
     </row>
-    <row r="2" ht="15" customHeight="1">
-      <c r="A2" t="s" s="6">
-        <v>4</v>
-      </c>
-      <c r="B2" s="7">
-        <v>0</v>
-      </c>
-      <c r="C2" s="7">
-        <v>14.04</v>
-      </c>
-      <c r="D2" s="7">
-        <v>0.8</v>
-      </c>
-      <c r="E2" s="7">
-        <v>0.27</v>
-      </c>
-      <c r="F2" s="8"/>
-      <c r="G2" s="5"/>
+    <row r="2" ht="30" customHeight="1">
+      <c r="A2" t="s" s="7">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s" s="8">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s" s="8">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s" s="8">
+        <v>7</v>
+      </c>
+      <c r="E2" t="s" s="8">
+        <v>8</v>
+      </c>
+      <c r="F2" t="s" s="8">
+        <v>9</v>
+      </c>
+      <c r="G2" s="4"/>
       <c r="H2" s="5"/>
       <c r="I2" s="5"/>
       <c r="J2" s="5"/>
@@ -1476,35 +1542,28 @@
       <c r="O2" s="5"/>
       <c r="P2" s="5"/>
       <c r="Q2" s="5"/>
-      <c r="R2" s="5"/>
-      <c r="S2" s="5"/>
-      <c r="T2" s="5"/>
-      <c r="U2" s="5"/>
-      <c r="V2" s="5"/>
-      <c r="W2" s="5"/>
-      <c r="X2" s="5"/>
-      <c r="Y2" s="5"/>
-      <c r="Z2" s="5"/>
-      <c r="AA2" s="5"/>
+      <c r="R2" s="9"/>
     </row>
-    <row r="3" ht="15" customHeight="1">
-      <c r="A3" t="s" s="9">
-        <v>5</v>
-      </c>
-      <c r="B3" s="10">
+    <row r="3" ht="30" customHeight="1">
+      <c r="A3" t="s" s="7">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s" s="8">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s" s="8">
+        <v>6</v>
+      </c>
+      <c r="D3" t="s" s="8">
+        <v>11</v>
+      </c>
+      <c r="E3" t="s" s="8">
+        <v>12</v>
+      </c>
+      <c r="F3" s="10">
         <v>0</v>
       </c>
-      <c r="C3" s="10">
-        <v>9.65</v>
-      </c>
-      <c r="D3" s="10">
-        <v>4.9</v>
-      </c>
-      <c r="E3" s="10">
-        <v>0</v>
-      </c>
-      <c r="F3" s="8"/>
-      <c r="G3" s="5"/>
+      <c r="G3" s="4"/>
       <c r="H3" s="5"/>
       <c r="I3" s="5"/>
       <c r="J3" s="5"/>
@@ -1515,35 +1574,28 @@
       <c r="O3" s="5"/>
       <c r="P3" s="5"/>
       <c r="Q3" s="5"/>
-      <c r="R3" s="5"/>
-      <c r="S3" s="5"/>
-      <c r="T3" s="5"/>
-      <c r="U3" s="5"/>
-      <c r="V3" s="5"/>
-      <c r="W3" s="5"/>
-      <c r="X3" s="5"/>
-      <c r="Y3" s="5"/>
-      <c r="Z3" s="5"/>
-      <c r="AA3" s="5"/>
+      <c r="R3" s="9"/>
     </row>
-    <row r="4" ht="15" customHeight="1">
-      <c r="A4" t="s" s="9">
+    <row r="4" ht="30" customHeight="1">
+      <c r="A4" t="s" s="7">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s" s="8">
         <v>6</v>
       </c>
-      <c r="B4" s="10">
-        <v>0</v>
-      </c>
-      <c r="C4" s="10">
-        <v>0.88</v>
-      </c>
-      <c r="D4" s="10">
-        <v>0</v>
+      <c r="C4" t="s" s="8">
+        <v>6</v>
+      </c>
+      <c r="D4" t="s" s="8">
+        <v>14</v>
       </c>
       <c r="E4" s="10">
         <v>0</v>
       </c>
-      <c r="F4" s="8"/>
-      <c r="G4" s="5"/>
+      <c r="F4" s="10">
+        <v>0</v>
+      </c>
+      <c r="G4" s="4"/>
       <c r="H4" s="5"/>
       <c r="I4" s="5"/>
       <c r="J4" s="5"/>
@@ -1554,35 +1606,28 @@
       <c r="O4" s="5"/>
       <c r="P4" s="5"/>
       <c r="Q4" s="5"/>
-      <c r="R4" s="5"/>
-      <c r="S4" s="5"/>
-      <c r="T4" s="5"/>
-      <c r="U4" s="5"/>
-      <c r="V4" s="5"/>
-      <c r="W4" s="5"/>
-      <c r="X4" s="5"/>
-      <c r="Y4" s="5"/>
-      <c r="Z4" s="5"/>
-      <c r="AA4" s="5"/>
+      <c r="R4" s="9"/>
     </row>
-    <row r="5" ht="15" customHeight="1">
-      <c r="A5" t="s" s="9">
-        <v>7</v>
-      </c>
-      <c r="B5" s="10">
-        <v>0</v>
-      </c>
-      <c r="C5" s="10">
-        <v>4.39</v>
-      </c>
-      <c r="D5" s="10">
-        <v>2.4</v>
-      </c>
-      <c r="E5" s="10">
-        <v>0.55</v>
-      </c>
-      <c r="F5" s="8"/>
-      <c r="G5" s="5"/>
+    <row r="5" ht="30" customHeight="1">
+      <c r="A5" t="s" s="7">
+        <v>15</v>
+      </c>
+      <c r="B5" t="s" s="8">
+        <v>6</v>
+      </c>
+      <c r="C5" t="s" s="8">
+        <v>6</v>
+      </c>
+      <c r="D5" t="s" s="8">
+        <v>16</v>
+      </c>
+      <c r="E5" t="s" s="8">
+        <v>17</v>
+      </c>
+      <c r="F5" t="s" s="8">
+        <v>18</v>
+      </c>
+      <c r="G5" s="4"/>
       <c r="H5" s="5"/>
       <c r="I5" s="5"/>
       <c r="J5" s="5"/>
@@ -1593,35 +1638,28 @@
       <c r="O5" s="5"/>
       <c r="P5" s="5"/>
       <c r="Q5" s="5"/>
-      <c r="R5" s="5"/>
-      <c r="S5" s="5"/>
-      <c r="T5" s="5"/>
-      <c r="U5" s="5"/>
-      <c r="V5" s="5"/>
-      <c r="W5" s="5"/>
-      <c r="X5" s="5"/>
-      <c r="Y5" s="5"/>
-      <c r="Z5" s="5"/>
-      <c r="AA5" s="5"/>
+      <c r="R5" s="9"/>
     </row>
-    <row r="6" ht="15" customHeight="1">
-      <c r="A6" t="s" s="9">
-        <v>8</v>
-      </c>
-      <c r="B6" s="10">
+    <row r="6" ht="30" customHeight="1">
+      <c r="A6" t="s" s="7">
+        <v>19</v>
+      </c>
+      <c r="B6" t="s" s="8">
+        <v>6</v>
+      </c>
+      <c r="C6" t="s" s="8">
+        <v>6</v>
+      </c>
+      <c r="D6" t="s" s="8">
+        <v>20</v>
+      </c>
+      <c r="E6" s="10">
         <v>0</v>
       </c>
-      <c r="C6" s="10">
-        <v>2.63</v>
-      </c>
-      <c r="D6" s="10">
-        <v>0</v>
-      </c>
-      <c r="E6" s="10">
-        <v>1.1</v>
-      </c>
-      <c r="F6" s="8"/>
-      <c r="G6" s="5"/>
+      <c r="F6" t="s" s="8">
+        <v>21</v>
+      </c>
+      <c r="G6" s="4"/>
       <c r="H6" s="5"/>
       <c r="I6" s="5"/>
       <c r="J6" s="5"/>
@@ -1632,35 +1670,28 @@
       <c r="O6" s="5"/>
       <c r="P6" s="5"/>
       <c r="Q6" s="5"/>
-      <c r="R6" s="5"/>
-      <c r="S6" s="5"/>
-      <c r="T6" s="5"/>
-      <c r="U6" s="5"/>
-      <c r="V6" s="5"/>
-      <c r="W6" s="5"/>
-      <c r="X6" s="5"/>
-      <c r="Y6" s="5"/>
-      <c r="Z6" s="5"/>
-      <c r="AA6" s="5"/>
+      <c r="R6" s="9"/>
     </row>
-    <row r="7" ht="15" customHeight="1">
-      <c r="A7" t="s" s="9">
-        <v>9</v>
-      </c>
-      <c r="B7" s="10">
-        <v>5.74</v>
-      </c>
-      <c r="C7" s="10">
-        <v>9.65</v>
-      </c>
-      <c r="D7" s="10">
-        <v>5.7</v>
-      </c>
-      <c r="E7" s="10">
-        <v>8.789999999999999</v>
-      </c>
-      <c r="F7" s="8"/>
-      <c r="G7" s="5"/>
+    <row r="7" ht="30" customHeight="1">
+      <c r="A7" t="s" s="7">
+        <v>22</v>
+      </c>
+      <c r="B7" t="s" s="8">
+        <v>23</v>
+      </c>
+      <c r="C7" t="s" s="8">
+        <v>24</v>
+      </c>
+      <c r="D7" t="s" s="8">
+        <v>11</v>
+      </c>
+      <c r="E7" t="s" s="8">
+        <v>25</v>
+      </c>
+      <c r="F7" t="s" s="8">
+        <v>26</v>
+      </c>
+      <c r="G7" s="4"/>
       <c r="H7" s="5"/>
       <c r="I7" s="5"/>
       <c r="J7" s="5"/>
@@ -1671,35 +1702,28 @@
       <c r="O7" s="5"/>
       <c r="P7" s="5"/>
       <c r="Q7" s="5"/>
-      <c r="R7" s="5"/>
-      <c r="S7" s="5"/>
-      <c r="T7" s="5"/>
-      <c r="U7" s="5"/>
-      <c r="V7" s="5"/>
-      <c r="W7" s="5"/>
-      <c r="X7" s="5"/>
-      <c r="Y7" s="5"/>
-      <c r="Z7" s="5"/>
-      <c r="AA7" s="5"/>
+      <c r="R7" s="11"/>
     </row>
-    <row r="8" ht="15" customHeight="1">
-      <c r="A8" t="s" s="9">
-        <v>10</v>
-      </c>
-      <c r="B8" s="10">
-        <v>0.36</v>
-      </c>
-      <c r="C8" s="10">
-        <v>5.26</v>
-      </c>
-      <c r="D8" s="10">
-        <v>0.8</v>
-      </c>
-      <c r="E8" s="10">
-        <v>0.82</v>
-      </c>
-      <c r="F8" s="8"/>
-      <c r="G8" s="5"/>
+    <row r="8" ht="30" customHeight="1">
+      <c r="A8" t="s" s="7">
+        <v>27</v>
+      </c>
+      <c r="B8" t="s" s="8">
+        <v>6</v>
+      </c>
+      <c r="C8" t="s" s="8">
+        <v>28</v>
+      </c>
+      <c r="D8" t="s" s="8">
+        <v>29</v>
+      </c>
+      <c r="E8" t="s" s="8">
+        <v>8</v>
+      </c>
+      <c r="F8" t="s" s="8">
+        <v>30</v>
+      </c>
+      <c r="G8" s="4"/>
       <c r="H8" s="5"/>
       <c r="I8" s="5"/>
       <c r="J8" s="5"/>
@@ -1710,35 +1734,28 @@
       <c r="O8" s="5"/>
       <c r="P8" s="5"/>
       <c r="Q8" s="5"/>
-      <c r="R8" s="5"/>
-      <c r="S8" s="5"/>
-      <c r="T8" s="5"/>
-      <c r="U8" s="5"/>
-      <c r="V8" s="5"/>
-      <c r="W8" s="5"/>
-      <c r="X8" s="5"/>
-      <c r="Y8" s="5"/>
-      <c r="Z8" s="5"/>
-      <c r="AA8" s="5"/>
+      <c r="R8" s="9"/>
     </row>
-    <row r="9" ht="15" customHeight="1">
-      <c r="A9" t="s" s="9">
-        <v>11</v>
-      </c>
-      <c r="B9" s="10">
-        <v>0</v>
-      </c>
-      <c r="C9" s="10">
-        <v>0.88</v>
-      </c>
-      <c r="D9" s="10">
-        <v>0.8</v>
-      </c>
-      <c r="E9" s="10">
-        <v>0.55</v>
-      </c>
-      <c r="F9" s="8"/>
-      <c r="G9" s="5"/>
+    <row r="9" ht="30" customHeight="1">
+      <c r="A9" t="s" s="7">
+        <v>31</v>
+      </c>
+      <c r="B9" t="s" s="8">
+        <v>6</v>
+      </c>
+      <c r="C9" t="s" s="8">
+        <v>6</v>
+      </c>
+      <c r="D9" t="s" s="8">
+        <v>14</v>
+      </c>
+      <c r="E9" t="s" s="8">
+        <v>8</v>
+      </c>
+      <c r="F9" t="s" s="8">
+        <v>18</v>
+      </c>
+      <c r="G9" s="4"/>
       <c r="H9" s="5"/>
       <c r="I9" s="5"/>
       <c r="J9" s="5"/>
@@ -1749,35 +1766,28 @@
       <c r="O9" s="5"/>
       <c r="P9" s="5"/>
       <c r="Q9" s="5"/>
-      <c r="R9" s="5"/>
-      <c r="S9" s="5"/>
-      <c r="T9" s="5"/>
-      <c r="U9" s="5"/>
-      <c r="V9" s="5"/>
-      <c r="W9" s="5"/>
-      <c r="X9" s="5"/>
-      <c r="Y9" s="5"/>
-      <c r="Z9" s="5"/>
-      <c r="AA9" s="5"/>
+      <c r="R9" s="9"/>
     </row>
-    <row r="10" ht="15" customHeight="1">
-      <c r="A10" t="s" s="9">
-        <v>12</v>
-      </c>
-      <c r="B10" s="10">
-        <v>7.66</v>
-      </c>
-      <c r="C10" s="10">
-        <v>3.51</v>
-      </c>
-      <c r="D10" s="10">
-        <v>1.6</v>
-      </c>
-      <c r="E10" s="10">
-        <v>8.52</v>
-      </c>
-      <c r="F10" s="8"/>
-      <c r="G10" s="5"/>
+    <row r="10" ht="30" customHeight="1">
+      <c r="A10" t="s" s="7">
+        <v>32</v>
+      </c>
+      <c r="B10" t="s" s="8">
+        <v>33</v>
+      </c>
+      <c r="C10" t="s" s="8">
+        <v>34</v>
+      </c>
+      <c r="D10" t="s" s="8">
+        <v>35</v>
+      </c>
+      <c r="E10" t="s" s="8">
+        <v>36</v>
+      </c>
+      <c r="F10" t="s" s="8">
+        <v>37</v>
+      </c>
+      <c r="G10" s="4"/>
       <c r="H10" s="5"/>
       <c r="I10" s="5"/>
       <c r="J10" s="5"/>
@@ -1788,35 +1798,28 @@
       <c r="O10" s="5"/>
       <c r="P10" s="5"/>
       <c r="Q10" s="5"/>
-      <c r="R10" s="5"/>
-      <c r="S10" s="5"/>
-      <c r="T10" s="5"/>
-      <c r="U10" s="5"/>
-      <c r="V10" s="5"/>
-      <c r="W10" s="5"/>
-      <c r="X10" s="5"/>
-      <c r="Y10" s="5"/>
-      <c r="Z10" s="5"/>
-      <c r="AA10" s="5"/>
+      <c r="R10" s="9"/>
     </row>
-    <row r="11" ht="15" customHeight="1">
-      <c r="A11" t="s" s="9">
-        <v>13</v>
-      </c>
-      <c r="B11" s="10">
-        <v>0.36</v>
-      </c>
-      <c r="C11" s="10">
+    <row r="11" ht="30" customHeight="1">
+      <c r="A11" t="s" s="7">
+        <v>38</v>
+      </c>
+      <c r="B11" t="s" s="8">
+        <v>39</v>
+      </c>
+      <c r="C11" t="s" s="8">
+        <v>6</v>
+      </c>
+      <c r="D11" s="10">
         <v>0</v>
       </c>
-      <c r="D11" s="10">
-        <v>0.8</v>
-      </c>
-      <c r="E11" s="10">
-        <v>0.82</v>
-      </c>
-      <c r="F11" s="8"/>
-      <c r="G11" s="5"/>
+      <c r="E11" t="s" s="8">
+        <v>8</v>
+      </c>
+      <c r="F11" t="s" s="8">
+        <v>30</v>
+      </c>
+      <c r="G11" s="4"/>
       <c r="H11" s="5"/>
       <c r="I11" s="5"/>
       <c r="J11" s="5"/>
@@ -1827,26 +1830,17 @@
       <c r="O11" s="5"/>
       <c r="P11" s="5"/>
       <c r="Q11" s="5"/>
-      <c r="R11" s="5"/>
-      <c r="S11" s="5"/>
-      <c r="T11" s="5"/>
-      <c r="U11" s="5"/>
-      <c r="V11" s="5"/>
-      <c r="W11" s="5"/>
-      <c r="X11" s="5"/>
-      <c r="Y11" s="5"/>
-      <c r="Z11" s="5"/>
-      <c r="AA11" s="5"/>
+      <c r="R11" s="9"/>
     </row>
-    <row r="12" ht="15" customHeight="1">
-      <c r="A12" t="s" s="9">
-        <v>14</v>
-      </c>
-      <c r="B12" s="10">
-        <v>0</v>
-      </c>
-      <c r="C12" s="10">
-        <v>0</v>
+    <row r="12" ht="30" customHeight="1">
+      <c r="A12" t="s" s="7">
+        <v>40</v>
+      </c>
+      <c r="B12" t="s" s="8">
+        <v>6</v>
+      </c>
+      <c r="C12" t="s" s="8">
+        <v>6</v>
       </c>
       <c r="D12" s="10">
         <v>0</v>
@@ -1854,8 +1848,10 @@
       <c r="E12" s="10">
         <v>0</v>
       </c>
-      <c r="F12" s="8"/>
-      <c r="G12" s="5"/>
+      <c r="F12" s="10">
+        <v>0</v>
+      </c>
+      <c r="G12" s="4"/>
       <c r="H12" s="5"/>
       <c r="I12" s="5"/>
       <c r="J12" s="5"/>
@@ -1866,35 +1862,28 @@
       <c r="O12" s="5"/>
       <c r="P12" s="5"/>
       <c r="Q12" s="5"/>
-      <c r="R12" s="5"/>
-      <c r="S12" s="5"/>
-      <c r="T12" s="5"/>
-      <c r="U12" s="5"/>
-      <c r="V12" s="5"/>
-      <c r="W12" s="5"/>
-      <c r="X12" s="5"/>
-      <c r="Y12" s="5"/>
-      <c r="Z12" s="5"/>
-      <c r="AA12" s="5"/>
+      <c r="R12" s="9"/>
     </row>
-    <row r="13" ht="15" customHeight="1">
-      <c r="A13" t="s" s="9">
-        <v>15</v>
-      </c>
-      <c r="B13" s="10">
-        <v>0.36</v>
-      </c>
-      <c r="C13" s="10">
+    <row r="13" ht="30" customHeight="1">
+      <c r="A13" t="s" s="7">
+        <v>41</v>
+      </c>
+      <c r="B13" t="s" s="8">
+        <v>6</v>
+      </c>
+      <c r="C13" t="s" s="8">
+        <v>28</v>
+      </c>
+      <c r="D13" s="10">
         <v>0</v>
       </c>
-      <c r="D13" s="10">
-        <v>2.4</v>
-      </c>
-      <c r="E13" s="10">
-        <v>1.92</v>
-      </c>
-      <c r="F13" s="8"/>
-      <c r="G13" s="5"/>
+      <c r="E13" t="s" s="8">
+        <v>17</v>
+      </c>
+      <c r="F13" t="s" s="8">
+        <v>33</v>
+      </c>
+      <c r="G13" s="4"/>
       <c r="H13" s="5"/>
       <c r="I13" s="5"/>
       <c r="J13" s="5"/>
@@ -1905,35 +1894,28 @@
       <c r="O13" s="5"/>
       <c r="P13" s="5"/>
       <c r="Q13" s="5"/>
-      <c r="R13" s="5"/>
-      <c r="S13" s="5"/>
-      <c r="T13" s="5"/>
-      <c r="U13" s="5"/>
-      <c r="V13" s="5"/>
-      <c r="W13" s="5"/>
-      <c r="X13" s="5"/>
-      <c r="Y13" s="5"/>
-      <c r="Z13" s="5"/>
-      <c r="AA13" s="5"/>
+      <c r="R13" s="9"/>
     </row>
-    <row r="14" ht="15" customHeight="1">
-      <c r="A14" t="s" s="9">
-        <v>16</v>
-      </c>
-      <c r="B14" s="10">
-        <v>1.09</v>
-      </c>
-      <c r="C14" s="10">
-        <v>1.75</v>
-      </c>
-      <c r="D14" s="10">
-        <v>12.2</v>
-      </c>
-      <c r="E14" s="10">
-        <v>8.24</v>
-      </c>
-      <c r="F14" s="8"/>
-      <c r="G14" s="5"/>
+    <row r="14" ht="30" customHeight="1">
+      <c r="A14" t="s" s="7">
+        <v>42</v>
+      </c>
+      <c r="B14" t="s" s="8">
+        <v>23</v>
+      </c>
+      <c r="C14" t="s" s="8">
+        <v>28</v>
+      </c>
+      <c r="D14" t="s" s="8">
+        <v>43</v>
+      </c>
+      <c r="E14" t="s" s="8">
+        <v>44</v>
+      </c>
+      <c r="F14" t="s" s="8">
+        <v>45</v>
+      </c>
+      <c r="G14" s="4"/>
       <c r="H14" s="5"/>
       <c r="I14" s="5"/>
       <c r="J14" s="5"/>
@@ -1944,35 +1926,28 @@
       <c r="O14" s="5"/>
       <c r="P14" s="5"/>
       <c r="Q14" s="5"/>
-      <c r="R14" s="5"/>
-      <c r="S14" s="5"/>
-      <c r="T14" s="5"/>
-      <c r="U14" s="5"/>
-      <c r="V14" s="5"/>
-      <c r="W14" s="5"/>
-      <c r="X14" s="5"/>
-      <c r="Y14" s="5"/>
-      <c r="Z14" s="5"/>
-      <c r="AA14" s="5"/>
+      <c r="R14" s="11"/>
     </row>
-    <row r="15" ht="15" customHeight="1">
-      <c r="A15" t="s" s="9">
-        <v>17</v>
-      </c>
-      <c r="B15" s="10">
-        <v>48.54</v>
-      </c>
-      <c r="C15" s="10">
-        <v>35.09</v>
-      </c>
-      <c r="D15" s="10">
-        <v>54.5</v>
-      </c>
-      <c r="E15" s="10">
-        <v>27.75</v>
-      </c>
-      <c r="F15" s="8"/>
-      <c r="G15" s="5"/>
+    <row r="15" ht="30" customHeight="1">
+      <c r="A15" t="s" s="7">
+        <v>46</v>
+      </c>
+      <c r="B15" t="s" s="8">
+        <v>47</v>
+      </c>
+      <c r="C15" t="s" s="8">
+        <v>48</v>
+      </c>
+      <c r="D15" t="s" s="8">
+        <v>49</v>
+      </c>
+      <c r="E15" t="s" s="8">
+        <v>50</v>
+      </c>
+      <c r="F15" t="s" s="8">
+        <v>51</v>
+      </c>
+      <c r="G15" s="4"/>
       <c r="H15" s="5"/>
       <c r="I15" s="5"/>
       <c r="J15" s="5"/>
@@ -1983,35 +1958,28 @@
       <c r="O15" s="5"/>
       <c r="P15" s="5"/>
       <c r="Q15" s="5"/>
-      <c r="R15" s="5"/>
-      <c r="S15" s="5"/>
-      <c r="T15" s="5"/>
-      <c r="U15" s="5"/>
-      <c r="V15" s="5"/>
-      <c r="W15" s="5"/>
-      <c r="X15" s="5"/>
-      <c r="Y15" s="5"/>
-      <c r="Z15" s="5"/>
-      <c r="AA15" s="5"/>
+      <c r="R15" s="9"/>
     </row>
-    <row r="16" ht="15" customHeight="1">
-      <c r="A16" t="s" s="9">
-        <v>18</v>
-      </c>
-      <c r="B16" s="10">
-        <v>7.3</v>
-      </c>
-      <c r="C16" s="10">
-        <v>11.4</v>
-      </c>
-      <c r="D16" s="10">
-        <v>4.9</v>
-      </c>
-      <c r="E16" s="10">
-        <v>5.22</v>
-      </c>
-      <c r="F16" s="8"/>
-      <c r="G16" s="5"/>
+    <row r="16" ht="30" customHeight="1">
+      <c r="A16" t="s" s="7">
+        <v>52</v>
+      </c>
+      <c r="B16" t="s" s="8">
+        <v>53</v>
+      </c>
+      <c r="C16" t="s" s="8">
+        <v>54</v>
+      </c>
+      <c r="D16" t="s" s="8">
+        <v>55</v>
+      </c>
+      <c r="E16" t="s" s="8">
+        <v>12</v>
+      </c>
+      <c r="F16" t="s" s="8">
+        <v>56</v>
+      </c>
+      <c r="G16" s="4"/>
       <c r="H16" s="5"/>
       <c r="I16" s="5"/>
       <c r="J16" s="5"/>
@@ -2022,35 +1990,28 @@
       <c r="O16" s="5"/>
       <c r="P16" s="5"/>
       <c r="Q16" s="5"/>
-      <c r="R16" s="5"/>
-      <c r="S16" s="5"/>
-      <c r="T16" s="5"/>
-      <c r="U16" s="5"/>
-      <c r="V16" s="5"/>
-      <c r="W16" s="5"/>
-      <c r="X16" s="5"/>
-      <c r="Y16" s="5"/>
-      <c r="Z16" s="5"/>
-      <c r="AA16" s="5"/>
+      <c r="R16" s="9"/>
     </row>
-    <row r="17" ht="15" customHeight="1">
-      <c r="A17" t="s" s="9">
-        <v>19</v>
-      </c>
-      <c r="B17" s="10">
-        <v>1.46</v>
-      </c>
-      <c r="C17" s="10">
-        <v>0.88</v>
-      </c>
-      <c r="D17" s="10">
-        <v>1.6</v>
-      </c>
-      <c r="E17" s="10">
-        <v>7.97</v>
-      </c>
-      <c r="F17" s="8"/>
-      <c r="G17" s="5"/>
+    <row r="17" ht="30" customHeight="1">
+      <c r="A17" t="s" s="7">
+        <v>57</v>
+      </c>
+      <c r="B17" t="s" s="8">
+        <v>6</v>
+      </c>
+      <c r="C17" t="s" s="8">
+        <v>58</v>
+      </c>
+      <c r="D17" t="s" s="8">
+        <v>14</v>
+      </c>
+      <c r="E17" t="s" s="8">
+        <v>36</v>
+      </c>
+      <c r="F17" t="s" s="8">
+        <v>59</v>
+      </c>
+      <c r="G17" s="4"/>
       <c r="H17" s="5"/>
       <c r="I17" s="5"/>
       <c r="J17" s="5"/>
@@ -2061,61 +2022,45 @@
       <c r="O17" s="5"/>
       <c r="P17" s="5"/>
       <c r="Q17" s="5"/>
-      <c r="R17" s="5"/>
-      <c r="S17" s="5"/>
-      <c r="T17" s="5"/>
-      <c r="U17" s="5"/>
-      <c r="V17" s="5"/>
-      <c r="W17" s="5"/>
-      <c r="X17" s="5"/>
-      <c r="Y17" s="5"/>
-      <c r="Z17" s="5"/>
-      <c r="AA17" s="5"/>
+      <c r="R17" s="9"/>
     </row>
-    <row r="18" ht="15" customHeight="1">
-      <c r="A18" t="s" s="9">
-        <v>20</v>
-      </c>
-      <c r="B18" s="10">
-        <v>27.37</v>
-      </c>
-      <c r="C18" s="10">
+    <row r="18" ht="30" customHeight="1">
+      <c r="A18" t="s" s="7">
+        <v>60</v>
+      </c>
+      <c r="B18" t="s" s="8">
+        <v>61</v>
+      </c>
+      <c r="C18" t="s" s="8">
+        <v>62</v>
+      </c>
+      <c r="D18" s="10">
         <v>0</v>
       </c>
-      <c r="D18" s="10">
-        <v>6.6</v>
-      </c>
-      <c r="E18" s="10">
-        <v>27.47</v>
-      </c>
-      <c r="F18" s="8"/>
-      <c r="G18" s="5"/>
+      <c r="E18" t="s" s="8">
+        <v>63</v>
+      </c>
+      <c r="F18" t="s" s="8">
+        <v>64</v>
+      </c>
+      <c r="G18" s="4"/>
       <c r="H18" s="5"/>
       <c r="I18" s="5"/>
       <c r="J18" s="5"/>
       <c r="K18" s="5"/>
-      <c r="L18" s="11"/>
+      <c r="L18" s="5"/>
       <c r="M18" s="5"/>
       <c r="N18" s="5"/>
       <c r="O18" s="5"/>
       <c r="P18" s="5"/>
       <c r="Q18" s="5"/>
-      <c r="R18" s="5"/>
-      <c r="S18" s="5"/>
-      <c r="T18" s="5"/>
-      <c r="U18" s="5"/>
-      <c r="V18" s="5"/>
-      <c r="W18" s="5"/>
-      <c r="X18" s="5"/>
-      <c r="Y18" s="5"/>
-      <c r="Z18" s="5"/>
-      <c r="AA18" s="5"/>
+      <c r="R18" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="92" useFirstPageNumber="0" orientation="landscape" pageOrder="downThenOver"/>
   <headerFooter>
-    <oddFooter>&amp;C&amp;"Helvetica,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added jupyter plugins to requirements and makefile
</commit_message>
<xml_diff>
--- a/symm_groups.xlsx
+++ b/symm_groups.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="30">
   <si>
     <t>Andalusia</t>
   </si>
@@ -25,7 +25,10 @@
     <t>Armenian</t>
   </si>
   <si>
-    <t>Seljuks</t>
+    <t>Rum Seljuks</t>
+  </si>
+  <si>
+    <t>Great Seljuks</t>
   </si>
   <si>
     <t>p1</t>
@@ -77,6 +80,27 @@
   </si>
   <si>
     <t>p6mm</t>
+  </si>
+  <si>
+    <t>Toplam</t>
+  </si>
+  <si>
+    <t>Adet</t>
+  </si>
+  <si>
+    <t>103 tane</t>
+  </si>
+  <si>
+    <t>225 tane</t>
+  </si>
+  <si>
+    <t>114tane</t>
+  </si>
+  <si>
+    <t>125tane</t>
+  </si>
+  <si>
+    <t>364tane</t>
   </si>
 </sst>
 </file>
@@ -326,7 +350,7 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -357,7 +381,7 @@
     <xf numFmtId="0" fontId="5" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="5" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="3" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="2" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -375,16 +399,25 @@
     <xf numFmtId="59" fontId="6" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
+    <xf numFmtId="0" fontId="3" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="2" fontId="5" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="5" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -1497,8 +1530,9 @@
     <col min="3" max="3" width="21.5" style="1" customWidth="1"/>
     <col min="4" max="4" width="29.1719" style="1" customWidth="1"/>
     <col min="5" max="5" width="19.6719" style="1" customWidth="1"/>
-    <col min="6" max="6" width="17.1719" style="1" customWidth="1"/>
-    <col min="7" max="8" width="7.35156" style="1" customWidth="1"/>
+    <col min="6" max="6" width="27.6719" style="1" customWidth="1"/>
+    <col min="7" max="7" width="21.1719" style="1" customWidth="1"/>
+    <col min="8" max="8" width="7.35156" style="1" customWidth="1"/>
     <col min="9" max="9" width="7.85156" style="1" customWidth="1"/>
     <col min="10" max="12" width="7.35156" style="1" customWidth="1"/>
     <col min="13" max="13" width="7.85156" style="1" customWidth="1"/>
@@ -1525,10 +1559,12 @@
       <c r="E1" t="s" s="3">
         <v>3</v>
       </c>
-      <c r="F1" t="s" s="4">
+      <c r="F1" t="s" s="3">
         <v>4</v>
       </c>
-      <c r="G1" s="5"/>
+      <c r="G1" t="s" s="4">
+        <v>5</v>
+      </c>
       <c r="H1" s="5"/>
       <c r="I1" s="5"/>
       <c r="J1" s="5"/>
@@ -1545,7 +1581,7 @@
     </row>
     <row r="2" ht="12.75" customHeight="1">
       <c r="A2" t="s" s="7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B2" s="8">
         <v>0.97</v>
@@ -1559,10 +1595,12 @@
       <c r="E2" s="9">
         <v>0.8</v>
       </c>
-      <c r="F2" s="10">
+      <c r="F2" s="9">
         <v>0.27</v>
       </c>
-      <c r="G2" s="5"/>
+      <c r="G2" s="10">
+        <v>0.8</v>
+      </c>
       <c r="H2" s="5"/>
       <c r="I2" s="5"/>
       <c r="J2" s="5"/>
@@ -1579,7 +1617,7 @@
     </row>
     <row r="3" ht="12.75" customHeight="1">
       <c r="A3" t="s" s="11">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B3" s="12">
         <v>0</v>
@@ -1593,10 +1631,12 @@
       <c r="E3" s="13">
         <v>4.9</v>
       </c>
-      <c r="F3" s="14">
+      <c r="F3" s="13">
         <v>0</v>
       </c>
-      <c r="G3" s="5"/>
+      <c r="G3" s="14">
+        <v>0</v>
+      </c>
       <c r="H3" s="5"/>
       <c r="I3" s="5"/>
       <c r="J3" s="5"/>
@@ -1613,7 +1653,7 @@
     </row>
     <row r="4" ht="12.75" customHeight="1">
       <c r="A4" t="s" s="11">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B4" s="12">
         <v>0</v>
@@ -1627,10 +1667,12 @@
       <c r="E4" s="13">
         <v>0</v>
       </c>
-      <c r="F4" s="14">
+      <c r="F4" s="13">
         <v>0</v>
       </c>
-      <c r="G4" s="5"/>
+      <c r="G4" s="16">
+        <v>0.8</v>
+      </c>
       <c r="H4" s="5"/>
       <c r="I4" s="5"/>
       <c r="J4" s="5"/>
@@ -1647,7 +1689,7 @@
     </row>
     <row r="5" ht="12.75" customHeight="1">
       <c r="A5" t="s" s="11">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B5" s="12">
         <v>0</v>
@@ -1661,10 +1703,12 @@
       <c r="E5" s="13">
         <v>2.4</v>
       </c>
-      <c r="F5" s="14">
+      <c r="F5" s="13">
         <v>0.55</v>
       </c>
-      <c r="G5" s="5"/>
+      <c r="G5" s="16">
+        <v>0</v>
+      </c>
       <c r="H5" s="5"/>
       <c r="I5" s="5"/>
       <c r="J5" s="5"/>
@@ -1681,7 +1725,7 @@
     </row>
     <row r="6" ht="12.75" customHeight="1">
       <c r="A6" t="s" s="11">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B6" s="12">
         <v>0.97</v>
@@ -1695,10 +1739,12 @@
       <c r="E6" s="13">
         <v>0</v>
       </c>
-      <c r="F6" s="14">
+      <c r="F6" s="13">
         <v>1.1</v>
       </c>
-      <c r="G6" s="5"/>
+      <c r="G6" s="16">
+        <v>2.4</v>
+      </c>
       <c r="H6" s="5"/>
       <c r="I6" s="5"/>
       <c r="J6" s="5"/>
@@ -1715,7 +1761,7 @@
     </row>
     <row r="7" ht="12.75" customHeight="1">
       <c r="A7" t="s" s="11">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B7" s="12">
         <v>1.942</v>
@@ -1729,10 +1775,12 @@
       <c r="E7" s="13">
         <v>5.7</v>
       </c>
-      <c r="F7" s="14">
+      <c r="F7" s="13">
         <v>8.789999999999999</v>
       </c>
-      <c r="G7" s="5"/>
+      <c r="G7" s="16">
+        <v>6.4</v>
+      </c>
       <c r="H7" s="5"/>
       <c r="I7" s="5"/>
       <c r="J7" s="5"/>
@@ -1749,7 +1797,7 @@
     </row>
     <row r="8" ht="12.75" customHeight="1">
       <c r="A8" t="s" s="11">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B8" s="12">
         <v>0</v>
@@ -1763,10 +1811,12 @@
       <c r="E8" s="13">
         <v>0.8</v>
       </c>
-      <c r="F8" s="14">
+      <c r="F8" s="13">
         <v>0.82</v>
       </c>
-      <c r="G8" s="5"/>
+      <c r="G8" s="16">
+        <v>0.8</v>
+      </c>
       <c r="H8" s="5"/>
       <c r="I8" s="5"/>
       <c r="J8" s="5"/>
@@ -1783,7 +1833,7 @@
     </row>
     <row r="9" ht="12.75" customHeight="1">
       <c r="A9" t="s" s="11">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B9" s="12">
         <v>0</v>
@@ -1797,10 +1847,12 @@
       <c r="E9" s="13">
         <v>0.8</v>
       </c>
-      <c r="F9" s="14">
+      <c r="F9" s="13">
         <v>0.55</v>
       </c>
-      <c r="G9" s="5"/>
+      <c r="G9" s="16">
+        <v>3.2</v>
+      </c>
       <c r="H9" s="5"/>
       <c r="I9" s="5"/>
       <c r="J9" s="5"/>
@@ -1817,7 +1869,7 @@
     </row>
     <row r="10" ht="12.75" customHeight="1">
       <c r="A10" t="s" s="11">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B10" s="12">
         <v>1.942</v>
@@ -1831,10 +1883,12 @@
       <c r="E10" s="13">
         <v>1.6</v>
       </c>
-      <c r="F10" s="14">
+      <c r="F10" s="13">
         <v>8.52</v>
       </c>
-      <c r="G10" s="5"/>
+      <c r="G10" s="16">
+        <v>11.2</v>
+      </c>
       <c r="H10" s="5"/>
       <c r="I10" s="5"/>
       <c r="J10" s="5"/>
@@ -1851,7 +1905,7 @@
     </row>
     <row r="11" ht="12.75" customHeight="1">
       <c r="A11" t="s" s="11">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B11" s="12">
         <v>0.97</v>
@@ -1865,10 +1919,12 @@
       <c r="E11" s="13">
         <v>0.8</v>
       </c>
-      <c r="F11" s="14">
+      <c r="F11" s="13">
         <v>0.82</v>
       </c>
-      <c r="G11" s="5"/>
+      <c r="G11" s="16">
+        <v>0</v>
+      </c>
       <c r="H11" s="5"/>
       <c r="I11" s="5"/>
       <c r="J11" s="5"/>
@@ -1885,7 +1941,7 @@
     </row>
     <row r="12" ht="12.75" customHeight="1">
       <c r="A12" t="s" s="11">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B12" s="12">
         <v>0</v>
@@ -1899,10 +1955,12 @@
       <c r="E12" s="13">
         <v>0</v>
       </c>
-      <c r="F12" s="14">
+      <c r="F12" s="13">
         <v>0</v>
       </c>
-      <c r="G12" s="5"/>
+      <c r="G12" s="16">
+        <v>0</v>
+      </c>
       <c r="H12" s="5"/>
       <c r="I12" s="5"/>
       <c r="J12" s="5"/>
@@ -1919,7 +1977,7 @@
     </row>
     <row r="13" ht="12.75" customHeight="1">
       <c r="A13" t="s" s="11">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B13" s="12">
         <v>0</v>
@@ -1933,10 +1991,12 @@
       <c r="E13" s="13">
         <v>2.4</v>
       </c>
-      <c r="F13" s="14">
+      <c r="F13" s="13">
         <v>1.92</v>
       </c>
-      <c r="G13" s="5"/>
+      <c r="G13" s="16">
+        <v>1.6</v>
+      </c>
       <c r="H13" s="5"/>
       <c r="I13" s="5"/>
       <c r="J13" s="5"/>
@@ -1953,7 +2013,7 @@
     </row>
     <row r="14" ht="12.75" customHeight="1">
       <c r="A14" t="s" s="11">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B14" s="12">
         <v>27.184</v>
@@ -1967,10 +2027,12 @@
       <c r="E14" s="13">
         <v>12.2</v>
       </c>
-      <c r="F14" s="14">
+      <c r="F14" s="13">
         <v>8.24</v>
       </c>
-      <c r="G14" s="5"/>
+      <c r="G14" s="16">
+        <v>9.6</v>
+      </c>
       <c r="H14" s="5"/>
       <c r="I14" s="5"/>
       <c r="J14" s="5"/>
@@ -1987,7 +2049,7 @@
     </row>
     <row r="15" ht="12.75" customHeight="1">
       <c r="A15" t="s" s="11">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B15" s="12">
         <v>51.46</v>
@@ -2001,10 +2063,12 @@
       <c r="E15" s="13">
         <v>54.5</v>
       </c>
-      <c r="F15" s="14">
+      <c r="F15" s="13">
         <v>27.75</v>
       </c>
-      <c r="G15" s="5"/>
+      <c r="G15" s="16">
+        <v>25.6</v>
+      </c>
       <c r="H15" s="5"/>
       <c r="I15" s="5"/>
       <c r="J15" s="5"/>
@@ -2021,7 +2085,7 @@
     </row>
     <row r="16" ht="12.75" customHeight="1">
       <c r="A16" t="s" s="11">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B16" s="12">
         <v>5.83</v>
@@ -2035,10 +2099,12 @@
       <c r="E16" s="13">
         <v>4.9</v>
       </c>
-      <c r="F16" s="14">
+      <c r="F16" s="13">
         <v>5.22</v>
       </c>
-      <c r="G16" s="5"/>
+      <c r="G16" s="16">
+        <v>12.8</v>
+      </c>
       <c r="H16" s="5"/>
       <c r="I16" s="5"/>
       <c r="J16" s="5"/>
@@ -2055,7 +2121,7 @@
     </row>
     <row r="17" ht="12.75" customHeight="1">
       <c r="A17" t="s" s="11">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B17" s="12">
         <v>2.91</v>
@@ -2069,10 +2135,12 @@
       <c r="E17" s="13">
         <v>1.6</v>
       </c>
-      <c r="F17" s="14">
+      <c r="F17" s="13">
         <v>7.97</v>
       </c>
-      <c r="G17" s="5"/>
+      <c r="G17" s="16">
+        <v>8</v>
+      </c>
       <c r="H17" s="5"/>
       <c r="I17" s="5"/>
       <c r="J17" s="5"/>
@@ -2089,7 +2157,7 @@
     </row>
     <row r="18" ht="12.75" customHeight="1">
       <c r="A18" t="s" s="11">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B18" s="12">
         <v>5.83</v>
@@ -2103,10 +2171,12 @@
       <c r="E18" s="13">
         <v>6.6</v>
       </c>
-      <c r="F18" s="14">
+      <c r="F18" s="13">
         <v>27.47</v>
       </c>
-      <c r="G18" s="5"/>
+      <c r="G18" s="16">
+        <v>18.8</v>
+      </c>
       <c r="H18" s="5"/>
       <c r="I18" s="5"/>
       <c r="J18" s="5"/>
@@ -2122,12 +2192,12 @@
       <c r="T18" s="5"/>
     </row>
     <row r="19" ht="24.75" customHeight="1">
-      <c r="A19" s="16"/>
-      <c r="B19" s="17"/>
-      <c r="C19" s="17"/>
-      <c r="D19" s="17"/>
-      <c r="E19" s="17"/>
-      <c r="F19" s="17"/>
+      <c r="A19" s="17"/>
+      <c r="B19" s="18"/>
+      <c r="C19" s="18"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="18"/>
       <c r="G19" s="5"/>
       <c r="H19" s="5"/>
       <c r="I19" s="5"/>
@@ -2144,13 +2214,33 @@
       <c r="T19" s="5"/>
     </row>
     <row r="20" ht="12.75" customHeight="1">
-      <c r="A20" s="16"/>
-      <c r="B20" s="18"/>
-      <c r="C20" s="18"/>
-      <c r="D20" s="17"/>
-      <c r="E20" s="17"/>
-      <c r="F20" s="17"/>
-      <c r="G20" s="5"/>
+      <c r="A20" t="s" s="19">
+        <v>23</v>
+      </c>
+      <c r="B20" s="20">
+        <f>SUM(B2:B18)</f>
+        <v>100.008</v>
+      </c>
+      <c r="C20" s="20">
+        <f>SUM(C2:C18)</f>
+        <v>99.994</v>
+      </c>
+      <c r="D20" s="21">
+        <f>SUM(D2:D18)</f>
+        <v>100.01</v>
+      </c>
+      <c r="E20" s="21">
+        <f>SUM(E2:E18)</f>
+        <v>100</v>
+      </c>
+      <c r="F20" s="21">
+        <f>SUM(F2:F18)</f>
+        <v>99.99000000000001</v>
+      </c>
+      <c r="G20" s="21">
+        <f>SUM(G2:G18)</f>
+        <v>102</v>
+      </c>
       <c r="H20" s="5"/>
       <c r="I20" s="5"/>
       <c r="J20" s="5"/>
@@ -2166,12 +2256,24 @@
       <c r="T20" s="5"/>
     </row>
     <row r="21" ht="12.75" customHeight="1">
-      <c r="A21" s="16"/>
-      <c r="B21" s="19"/>
-      <c r="C21" s="19"/>
-      <c r="D21" s="19"/>
-      <c r="E21" s="19"/>
-      <c r="F21" s="19"/>
+      <c r="A21" t="s" s="19">
+        <v>24</v>
+      </c>
+      <c r="B21" t="s" s="22">
+        <v>25</v>
+      </c>
+      <c r="C21" t="s" s="22">
+        <v>26</v>
+      </c>
+      <c r="D21" t="s" s="22">
+        <v>27</v>
+      </c>
+      <c r="E21" t="s" s="22">
+        <v>28</v>
+      </c>
+      <c r="F21" t="s" s="22">
+        <v>29</v>
+      </c>
       <c r="G21" s="5"/>
       <c r="H21" s="5"/>
       <c r="I21" s="5"/>
@@ -2320,25 +2422,25 @@
       <c r="T27" s="5"/>
     </row>
     <row r="28" ht="12.75" customHeight="1">
-      <c r="A28" s="20"/>
-      <c r="B28" s="20"/>
-      <c r="C28" s="20"/>
-      <c r="D28" s="20"/>
-      <c r="E28" s="20"/>
-      <c r="F28" s="20"/>
-      <c r="G28" s="20"/>
-      <c r="H28" s="20"/>
-      <c r="I28" s="20"/>
-      <c r="J28" s="20"/>
-      <c r="K28" s="20"/>
-      <c r="L28" s="20"/>
-      <c r="M28" s="20"/>
-      <c r="N28" s="20"/>
-      <c r="O28" s="20"/>
-      <c r="P28" s="20"/>
-      <c r="Q28" s="20"/>
-      <c r="R28" s="21"/>
-      <c r="S28" s="22"/>
+      <c r="A28" s="23"/>
+      <c r="B28" s="23"/>
+      <c r="C28" s="23"/>
+      <c r="D28" s="23"/>
+      <c r="E28" s="23"/>
+      <c r="F28" s="23"/>
+      <c r="G28" s="23"/>
+      <c r="H28" s="23"/>
+      <c r="I28" s="23"/>
+      <c r="J28" s="23"/>
+      <c r="K28" s="23"/>
+      <c r="L28" s="23"/>
+      <c r="M28" s="23"/>
+      <c r="N28" s="23"/>
+      <c r="O28" s="23"/>
+      <c r="P28" s="23"/>
+      <c r="Q28" s="23"/>
+      <c r="R28" s="24"/>
+      <c r="S28" s="25"/>
       <c r="T28" s="5"/>
     </row>
     <row r="29" ht="12.75" customHeight="1">
@@ -2348,39 +2450,39 @@
       <c r="D29" s="5"/>
       <c r="E29" s="5"/>
       <c r="F29" s="5"/>
-      <c r="G29" s="23"/>
+      <c r="G29" s="26"/>
       <c r="H29" s="5"/>
-      <c r="I29" s="23"/>
-      <c r="J29" s="23"/>
-      <c r="K29" s="23"/>
-      <c r="L29" s="23"/>
-      <c r="M29" s="23"/>
-      <c r="N29" s="23"/>
-      <c r="O29" s="23"/>
-      <c r="P29" s="23"/>
-      <c r="Q29" s="23"/>
-      <c r="R29" s="23"/>
-      <c r="S29" s="24"/>
-      <c r="T29" s="25"/>
+      <c r="I29" s="26"/>
+      <c r="J29" s="26"/>
+      <c r="K29" s="26"/>
+      <c r="L29" s="26"/>
+      <c r="M29" s="26"/>
+      <c r="N29" s="26"/>
+      <c r="O29" s="26"/>
+      <c r="P29" s="26"/>
+      <c r="Q29" s="26"/>
+      <c r="R29" s="26"/>
+      <c r="S29" s="27"/>
+      <c r="T29" s="28"/>
     </row>
     <row r="30" ht="12.75" customHeight="1">
-      <c r="A30" s="20"/>
-      <c r="B30" s="20"/>
-      <c r="C30" s="20"/>
-      <c r="D30" s="20"/>
-      <c r="E30" s="20"/>
-      <c r="F30" s="20"/>
-      <c r="G30" s="20"/>
-      <c r="H30" s="20"/>
-      <c r="I30" s="20"/>
-      <c r="J30" s="20"/>
-      <c r="K30" s="20"/>
-      <c r="L30" s="20"/>
-      <c r="M30" s="20"/>
-      <c r="N30" s="20"/>
-      <c r="O30" s="20"/>
-      <c r="P30" s="20"/>
-      <c r="Q30" s="20"/>
+      <c r="A30" s="23"/>
+      <c r="B30" s="23"/>
+      <c r="C30" s="23"/>
+      <c r="D30" s="23"/>
+      <c r="E30" s="23"/>
+      <c r="F30" s="23"/>
+      <c r="G30" s="23"/>
+      <c r="H30" s="23"/>
+      <c r="I30" s="23"/>
+      <c r="J30" s="23"/>
+      <c r="K30" s="23"/>
+      <c r="L30" s="23"/>
+      <c r="M30" s="23"/>
+      <c r="N30" s="23"/>
+      <c r="O30" s="23"/>
+      <c r="P30" s="23"/>
+      <c r="Q30" s="23"/>
       <c r="R30" s="5"/>
       <c r="S30" s="6"/>
       <c r="T30" s="5"/>

</xml_diff>